<commit_message>
Add overview tables for omics analysis tools
</commit_message>
<xml_diff>
--- a/docs/source/index/tables/t0_mapper.xlsx
+++ b/docs/source/index/tables/t0_mapper.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -38,6 +38,24 @@
   </si>
   <si>
     <t xml:space="preserve">aa.load_dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t2_omics_analysis_tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analysis tools for omics data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t3_omics_post-analysis_tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post-analysis tools for omics data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t4_gene_enrichment_tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gene enrichment analysis tools</t>
   </si>
 </sst>
 </file>
@@ -161,13 +179,13 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="11.52"/>
   </cols>
@@ -195,14 +213,30 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
First version of cImpute tutorial
</commit_message>
<xml_diff>
--- a/docs/source/index/tables/t0_mapper.xlsx
+++ b/docs/source/index/tables/t0_mapper.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Analysis tools for omics data</t>
   </si>
   <si>
-    <t xml:space="preserve">t3_omics_post-analysis_tools</t>
+    <t xml:space="preserve">t3_omics_post_analysis_tools</t>
   </si>
   <si>
     <t xml:space="preserve">Post-analysis tools for omics data</t>
@@ -179,10 +179,10 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.98"/>

</xml_diff>

<commit_message>
Update load_dataset and add use-case datasets
</commit_message>
<xml_diff>
--- a/docs/source/index/tables/t0_mapper.xlsx
+++ b/docs/source/index/tables/t0_mapper.xlsx
@@ -31,10 +31,10 @@
     <t xml:space="preserve">See Also</t>
   </si>
   <si>
-    <t xml:space="preserve">t1_overview_proteomics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proteomic example datasets</t>
+    <t xml:space="preserve">t1_overview_datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omics example datasets</t>
   </si>
   <si>
     <t xml:space="preserve">aa.load_dataset</t>
@@ -179,10 +179,10 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.98"/>

</xml_diff>

<commit_message>
Add omics fields and quantification methods tables to ducmentation
</commit_message>
<xml_diff>
--- a/docs/source/index/tables/t0_mapper.xlsx
+++ b/docs/source/index/tables/t0_mapper.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -31,7 +31,19 @@
     <t xml:space="preserve">See Also</t>
   </si>
   <si>
-    <t xml:space="preserve">t1_overview_datasets</t>
+    <t xml:space="preserve">t1_omics_fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omic fields targeted by xOmics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t2_quantification_methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantification methods used in omic fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t3_overview_datasets</t>
   </si>
   <si>
     <t xml:space="preserve">Omics example datasets</t>
@@ -40,22 +52,22 @@
     <t xml:space="preserve">aa.load_dataset</t>
   </si>
   <si>
-    <t xml:space="preserve">t2_omics_analysis_tools</t>
+    <t xml:space="preserve">t4_omics_analysis_tools</t>
   </si>
   <si>
     <t xml:space="preserve">Analysis tools for omics data</t>
   </si>
   <si>
-    <t xml:space="preserve">t3_omics_post_analysis_tools</t>
+    <t xml:space="preserve">t5_omics_post_analysis_tools</t>
   </si>
   <si>
     <t xml:space="preserve">Post-analysis tools for omics data</t>
   </si>
   <si>
-    <t xml:space="preserve">t4_gene_enrichment_tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gene enrichment analysis tools</t>
+    <t xml:space="preserve">t6_enrichment_tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrichment analysis tools</t>
   </si>
 </sst>
 </file>
@@ -146,13 +158,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -179,10 +195,10 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.98"/>
@@ -202,75 +218,88 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2"/>
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>